<commit_message>
Ajustes na planilha de riscos
</commit_message>
<xml_diff>
--- a/documents/xlsx/planilha_de_riscos.xlsx
+++ b/documents/xlsx/planilha_de_riscos.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakar\Desktop\BandTec\Primeiro semestre\Iniciativa 0\Iniciativa-0\documents\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="8520"/>
+    <workbookView xWindow="480" yWindow="720" windowWidth="18195" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,29 +21,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
-  <si>
-    <t>Planilia de Riscos</t>
-  </si>
-  <si>
-    <t>Codigo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>Risco</t>
   </si>
   <si>
-    <t>Um integrante acabou saindo.</t>
-  </si>
-  <si>
-    <t>Intriga interna no grupo</t>
-  </si>
-  <si>
-    <t>Intregrante debilitado</t>
-  </si>
-  <si>
-    <t>O integrante teve problemas  internos</t>
-  </si>
-  <si>
     <t>Acabar a luz de um dos integrantes</t>
   </si>
   <si>
@@ -48,12 +35,6 @@
     <t>O computador de um dos integrantes parar de funcionar</t>
   </si>
   <si>
-    <t>Acabar tendo de trocar o tema do projeto</t>
-  </si>
-  <si>
-    <t>Não ter o projeto concluido</t>
-  </si>
-  <si>
     <t>Perda de comunicação entre os integrantes da equipe</t>
   </si>
   <si>
@@ -85,12 +66,73 @@
   </si>
   <si>
     <t>Mitigar</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Planilha de Riscos - Tolerante ao risco</t>
+  </si>
+  <si>
+    <t>Como?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazer reunião de alinhamento para reajustar as tarefas que estavam em responsabilidade do membro que saiu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ter reuniões de grupo para feedbacks abertos e ajustes de desavenças. 
+</t>
+  </si>
+  <si>
+    <t>Integrante debilitado / doente</t>
+  </si>
+  <si>
+    <t>Incentivar o membro a cuidar da saúde, e incentivar os demais membros a cuidarem da saúde para prevenir doenças.</t>
+  </si>
+  <si>
+    <t>Intrigas internas no grupo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar o prazo da tarefa em execução, se estiver com o prazo curto, remanejar para que outro membro conclua. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fazendo reunião de ajuste com todos do grupo junto com uma sprint backlog para definir novos prazos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reunir todos os membros do grupo para reforçar os itens essenciais que devem ser entregues e aumentar o tempo de trabalho no projeto. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reunião de alinhamento do grupo, e definir um lider para tomar a frente do grupo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manter o repositorio na nuvem (GITHUB) e pelo menos 2 integrantes do grupo ter o repositorio atualizado no pc. </t>
+  </si>
+  <si>
+    <t>Definir que todos os integrantes devem ter um backup atualizado do projeto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar testes em diferentes sistemas uma semana antes da apresentação do projeto. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar ensaios com todos os integrantes invertendo os papeis de apresentação, para que todos saibam apresentar o projeto por completo. </t>
+  </si>
+  <si>
+    <t>O integrante teve problemas  internos ????</t>
+  </si>
+  <si>
+    <t>Um integrante poderá sair do projeto.</t>
+  </si>
+  <si>
+    <t>Acabar tendo que trocar o tema do projeto</t>
+  </si>
+  <si>
+    <t>Não ter o projeto concluído</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,12 +177,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -152,43 +194,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -237,37 +242,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -276,18 +269,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -299,6 +307,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -306,7 +317,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -344,9 +355,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -381,7 +392,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,7 +427,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -592,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +615,7 @@
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:12" x14ac:dyDescent="0.25">
@@ -615,236 +627,254 @@
     </row>
     <row r="3" spans="3:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
-      <c r="D3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="1"/>
+      <c r="D3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="3:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
-      <c r="D4" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="11" t="s">
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
-      <c r="D5" s="10">
-        <v>1</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="10">
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="6">
         <v>2</v>
       </c>
-      <c r="G5" s="10">
-        <v>3</v>
-      </c>
-      <c r="H5" s="10">
+      <c r="G5" s="6">
+        <v>3</v>
+      </c>
+      <c r="H5" s="6">
         <v>6</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="1"/>
+      <c r="I5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
-      <c r="D6" s="9">
+      <c r="D6" s="5">
         <v>2</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="9">
-        <v>1</v>
-      </c>
-      <c r="G6" s="9">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
         <v>2</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="5">
         <v>2</v>
       </c>
-      <c r="I6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="1"/>
+      <c r="I6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
-      <c r="D7" s="10">
-        <v>3</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="10">
-        <v>1</v>
-      </c>
-      <c r="G7" s="10">
-        <v>3</v>
-      </c>
-      <c r="H7" s="10">
-        <v>3</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="1"/>
+      <c r="D7" s="6">
+        <v>3</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>3</v>
+      </c>
+      <c r="H7" s="6">
+        <v>3</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
-      <c r="D8" s="9">
+      <c r="D8" s="5">
         <v>4</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="E8" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="18">
         <v>2</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="18">
         <v>2</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="18">
         <v>4</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="1"/>
+      <c r="I8" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="19"/>
     </row>
     <row r="9" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
-      <c r="D9" s="10">
+      <c r="D9" s="6">
         <v>5</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="10">
-        <v>1</v>
-      </c>
-      <c r="G9" s="10">
-        <v>1</v>
-      </c>
-      <c r="H9" s="10">
-        <v>1</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="1"/>
+      <c r="E9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
-      <c r="D10" s="9">
+      <c r="D10" s="5">
         <v>6</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="9">
-        <v>3</v>
-      </c>
-      <c r="G10" s="9">
-        <v>1</v>
-      </c>
-      <c r="H10" s="9">
-        <v>3</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>3</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5">
+        <v>3</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
-      <c r="D11" s="10">
+      <c r="D11" s="6">
         <v>7</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="10">
+      <c r="E11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="6">
         <v>2</v>
       </c>
-      <c r="G11" s="10">
-        <v>3</v>
-      </c>
-      <c r="H11" s="10">
+      <c r="G11" s="6">
+        <v>3</v>
+      </c>
+      <c r="H11" s="6">
         <v>6</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="1"/>
+      <c r="I11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
-      <c r="D12" s="9">
+      <c r="D12" s="5">
         <v>8</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9">
-        <v>3</v>
-      </c>
-      <c r="H12" s="9">
-        <v>3</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>3</v>
+      </c>
+      <c r="H12" s="5">
+        <v>3</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
-      <c r="D13" s="10">
+      <c r="D13" s="6">
         <v>9</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="10">
-        <v>1</v>
-      </c>
-      <c r="G13" s="10">
-        <v>3</v>
-      </c>
-      <c r="H13" s="10">
-        <v>3</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="1"/>
+      <c r="E13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6">
+        <v>3</v>
+      </c>
+      <c r="H13" s="6">
+        <v>3</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
@@ -852,7 +882,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
@@ -863,32 +893,36 @@
       <c r="H14" s="2">
         <v>3</v>
       </c>
-      <c r="I14" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="1"/>
+      <c r="I14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
-      <c r="D15" s="10">
+      <c r="D15" s="6">
         <v>11</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6">
+        <v>2</v>
+      </c>
+      <c r="H15" s="6">
+        <v>2</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="10">
-        <v>1</v>
-      </c>
-      <c r="G15" s="10">
-        <v>2</v>
-      </c>
-      <c r="H15" s="10">
-        <v>2</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="1"/>
+      <c r="J15" s="16" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
@@ -896,7 +930,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
@@ -907,61 +941,67 @@
       <c r="H16" s="2">
         <v>1</v>
       </c>
-      <c r="I16" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="1"/>
+      <c r="I16" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="17" spans="3:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
-      <c r="D17" s="10">
+      <c r="D17" s="6">
         <v>13</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="10">
-        <v>1</v>
-      </c>
-      <c r="G17" s="10">
-        <v>1</v>
-      </c>
-      <c r="H17" s="10">
-        <v>1</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="3:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
-      <c r="D18" s="11">
+      <c r="D18" s="7">
         <v>14</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="11">
+      <c r="E18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="7">
         <v>2</v>
       </c>
-      <c r="G18" s="11">
-        <v>3</v>
-      </c>
-      <c r="H18" s="11">
+      <c r="G18" s="7">
+        <v>3</v>
+      </c>
+      <c r="H18" s="7">
         <v>6</v>
       </c>
-      <c r="I18" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="1"/>
+      <c r="I18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I28" s="15"/>
+      <c r="I28" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="D3:J3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Correção planilha de Riscos e Analytics
</commit_message>
<xml_diff>
--- a/documents/xlsx/planilha_de_riscos.xlsx
+++ b/documents/xlsx/planilha_de_riscos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakar\Desktop\BandTec\Primeiro semestre\Iniciativa 0\Iniciativa-0\documents\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakar\Desktop\BandTec\Primeiro semestre\Iniciativa 0\startech\documents\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="720" windowWidth="18195" windowHeight="8520"/>
+    <workbookView xWindow="480" yWindow="1320" windowWidth="18195" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>Risco</t>
   </si>
@@ -117,9 +117,6 @@
     <t xml:space="preserve">Realizar ensaios com todos os integrantes invertendo os papeis de apresentação, para que todos saibam apresentar o projeto por completo. </t>
   </si>
   <si>
-    <t>O integrante teve problemas  internos ????</t>
-  </si>
-  <si>
     <t>Um integrante poderá sair do projeto.</t>
   </si>
   <si>
@@ -127,6 +124,12 @@
   </si>
   <si>
     <t>Não ter o projeto concluído</t>
+  </si>
+  <si>
+    <t>O integrante teve problemas  pessoais</t>
+  </si>
+  <si>
+    <t>O integrante deverá comunicar o grupo para que tanto ele quanto o grupo se adeque a nova situação.</t>
   </si>
 </sst>
 </file>
@@ -156,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,12 +175,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -276,25 +273,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -603,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,15 +612,15 @@
     </row>
     <row r="3" spans="3:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="3:12" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
@@ -667,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="6">
         <v>2</v>
@@ -681,7 +666,7 @@
       <c r="I5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="13" t="s">
         <v>18</v>
       </c>
     </row>
@@ -702,14 +687,14 @@
       <c r="H6" s="5">
         <v>2</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="6">
         <v>3</v>
@@ -729,7 +714,7 @@
       <c r="I7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="13" t="s">
         <v>21</v>
       </c>
       <c r="L7" s="1"/>
@@ -739,22 +724,24 @@
       <c r="D8" s="5">
         <v>4</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="18">
+      <c r="E8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="5">
         <v>2</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="5">
         <v>2</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="5">
         <v>4</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="19"/>
+      <c r="J8" s="15" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="3:12" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
@@ -776,7 +763,7 @@
       <c r="I9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -797,10 +784,10 @@
       <c r="H10" s="5">
         <v>3</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="15" t="s">
         <v>23</v>
       </c>
     </row>
@@ -824,7 +811,7 @@
       <c r="I11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="13" t="s">
         <v>23</v>
       </c>
     </row>
@@ -834,7 +821,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="5">
         <v>1</v>
@@ -845,10 +832,10 @@
       <c r="H12" s="5">
         <v>3</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -858,7 +845,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="6">
         <v>1</v>
@@ -872,7 +859,7 @@
       <c r="I13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="J13" s="13" t="s">
         <v>25</v>
       </c>
     </row>
@@ -893,10 +880,10 @@
       <c r="H14" s="2">
         <v>3</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="15" t="s">
         <v>26</v>
       </c>
     </row>
@@ -920,7 +907,7 @@
       <c r="I15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="J15" s="13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -941,10 +928,10 @@
       <c r="H16" s="2">
         <v>1</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="16" t="s">
+      <c r="J16" s="15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -968,7 +955,7 @@
       <c r="I17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="J17" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -989,10 +976,10 @@
       <c r="H18" s="7">
         <v>6</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="15" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>